<commit_message>
Adding a code base with exercise modules and sample. Adding data. Updating schedule, and exercises.
</commit_message>
<xml_diff>
--- a/Intro to Apache Spark Schedule.xlsx
+++ b/Intro to Apache Spark Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-10140" windowWidth="19200" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="-29340" yWindow="-7420" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <r>
       <rPr>
@@ -47,6 +47,93 @@
     </r>
   </si>
   <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>TOPIC</t>
+  </si>
+  <si>
+    <t>Apache Spark History/Background and MapReduce</t>
+  </si>
+  <si>
+    <t>System Setup</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Exercise 2 - Joining Datasets</t>
+  </si>
+  <si>
+    <t>Advanced Apache Spark APIs</t>
+  </si>
+  <si>
+    <t>Shared Variables</t>
+  </si>
+  <si>
+    <t>Exercise 3 - Shared Variables</t>
+  </si>
+  <si>
+    <t>Misc. Concepts</t>
+  </si>
+  <si>
+    <t>Q&amp;A</t>
+  </si>
+  <si>
+    <t>9:00 - 9:45</t>
+  </si>
+  <si>
+    <t>9:45 - 10:00</t>
+  </si>
+  <si>
+    <t>11:00 - 11:30</t>
+  </si>
+  <si>
+    <t>1:30 - 2:00</t>
+  </si>
+  <si>
+    <t>2:00 - 2:30</t>
+  </si>
+  <si>
+    <t>2:30 - 2:45</t>
+  </si>
+  <si>
+    <t>2:45 - 3:00</t>
+  </si>
+  <si>
+    <t>3:00 - 3:30</t>
+  </si>
+  <si>
+    <t>3:30 - 4:00</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sponsored by: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Clairvoyant</t>
+    </r>
+  </si>
+  <si>
+    <t>4:00 - 4:30</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>Intro to Apache Spark Workshop</t>
+  </si>
+  <si>
+    <t>Exercise 4 - Spark Submit</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -71,114 +158,39 @@
  - Introduce the Apache Spark EcoSystem
  - Provide an in depth look at Core Apache Spark
          - Implementation
-         API’s
-         Fault Tolerance
-         RDDs
+         - API’s
+         - Fault Tolerance
+         - RDDs
  - Give you experience with Apache Spark through examples and exercises
 </t>
     </r>
   </si>
   <si>
-    <t>TIME</t>
-  </si>
-  <si>
-    <t>TOPIC</t>
-  </si>
-  <si>
-    <t>Apache Spark History/Background and MapReduce</t>
-  </si>
-  <si>
-    <t>System Setup</t>
-  </si>
-  <si>
-    <t>Lunch</t>
-  </si>
-  <si>
-    <t>Exercise 1 - Access Logs</t>
-  </si>
-  <si>
-    <t>Exercise 2 - Joining Datasets</t>
-  </si>
-  <si>
-    <t>Apache Spark RDDs and API's</t>
-  </si>
-  <si>
-    <t>Advanced Apache Spark APIs</t>
-  </si>
-  <si>
-    <t>Shared Variables</t>
-  </si>
-  <si>
-    <t>Exercise 3 - Shared Variables</t>
-  </si>
-  <si>
-    <t>Misc. Concepts</t>
-  </si>
-  <si>
-    <t>Q&amp;A</t>
-  </si>
-  <si>
-    <t>9:00 - 9:45</t>
-  </si>
-  <si>
-    <t>9:45 - 10:00</t>
-  </si>
-  <si>
-    <t>10:00 - 11:00</t>
-  </si>
-  <si>
-    <t>11:00 - 11:30</t>
-  </si>
-  <si>
-    <t>11:30 - 12:30</t>
-  </si>
-  <si>
-    <t>12:30 - 1:30</t>
-  </si>
-  <si>
-    <t>1:30 - 2:00</t>
-  </si>
-  <si>
-    <t>2:00 - 2:30</t>
-  </si>
-  <si>
-    <t>2:30 - 2:45</t>
-  </si>
-  <si>
-    <t>2:45 - 3:00</t>
-  </si>
-  <si>
-    <t>3:00 - 3:30</t>
-  </si>
-  <si>
-    <t>3:30 - 4:00</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sponsored by: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Clairvoyant</t>
-    </r>
-  </si>
-  <si>
-    <t>4:00 - 4:30</t>
-  </si>
-  <si>
-    <t>Break</t>
-  </si>
-  <si>
-    <t>Intro to Apache Spark Workshop</t>
-  </si>
-  <si>
-    <t>Exercise 4 - Spark Submit</t>
+    <t>Apache Spark Context and RDDs</t>
+  </si>
+  <si>
+    <t>Apache Spark APIs</t>
+  </si>
+  <si>
+    <t>10:00 - 10:30</t>
+  </si>
+  <si>
+    <t>10:30 - 11:00</t>
+  </si>
+  <si>
+    <t>11:30 - 12:00</t>
+  </si>
+  <si>
+    <t>12:00 - 1:00</t>
+  </si>
+  <si>
+    <t>1:00 - 1:30</t>
+  </si>
+  <si>
+    <t>Exercise 2 - Access Logs</t>
+  </si>
+  <si>
+    <t>Exercise 1 - Running Spark Jobs</t>
   </si>
 </sst>
 </file>
@@ -313,7 +325,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -334,41 +346,46 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -378,6 +395,7 @@
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -388,6 +406,7 @@
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -717,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -729,178 +748,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="41" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1">
-      <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="3"/>
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" ht="87" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:3" ht="173" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" ht="25" customHeight="1">
       <c r="A5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="29" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29" customHeight="1">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:3" ht="29" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="29" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="29" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="29" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="29" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="29" customHeight="1">
+      <c r="A12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="29" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29" customHeight="1">
+      <c r="A14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="29" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="29" customHeight="1">
+      <c r="A15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="29" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="29" customHeight="1">
+      <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="29" customHeight="1">
-      <c r="A9" s="4" t="s">
+    <row r="17" spans="1:3" ht="29" customHeight="1">
+      <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="29" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="29" customHeight="1">
+      <c r="A18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="29" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="29" customHeight="1">
+      <c r="A19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="29" customHeight="1">
-      <c r="A12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="29" customHeight="1">
-      <c r="A13" s="8" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="29" customHeight="1">
+      <c r="A20" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="29" customHeight="1">
-      <c r="A14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="29" customHeight="1">
-      <c r="A15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="29" customHeight="1">
-      <c r="A16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="29" customHeight="1">
-      <c r="A17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="29" customHeight="1">
-      <c r="A18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Adding final slides and updating schedule. Also modifying the load-files-to-vm.sh file.
</commit_message>
<xml_diff>
--- a/Intro to Apache Spark Schedule.xlsx
+++ b/Intro to Apache Spark Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-29340" yWindow="-7420" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <r>
       <rPr>
@@ -62,49 +62,19 @@
     <t>Lunch</t>
   </si>
   <si>
-    <t>Exercise 2 - Joining Datasets</t>
-  </si>
-  <si>
-    <t>Advanced Apache Spark APIs</t>
-  </si>
-  <si>
     <t>Shared Variables</t>
   </si>
   <si>
-    <t>Exercise 3 - Shared Variables</t>
-  </si>
-  <si>
     <t>Misc. Concepts</t>
   </si>
   <si>
     <t>Q&amp;A</t>
   </si>
   <si>
-    <t>9:00 - 9:45</t>
-  </si>
-  <si>
-    <t>9:45 - 10:00</t>
-  </si>
-  <si>
-    <t>11:00 - 11:30</t>
-  </si>
-  <si>
     <t>1:30 - 2:00</t>
   </si>
   <si>
     <t>2:00 - 2:30</t>
-  </si>
-  <si>
-    <t>2:30 - 2:45</t>
-  </si>
-  <si>
-    <t>2:45 - 3:00</t>
-  </si>
-  <si>
-    <t>3:00 - 3:30</t>
-  </si>
-  <si>
-    <t>3:30 - 4:00</t>
   </si>
   <si>
     <r>
@@ -125,13 +95,7 @@
     <t>4:00 - 4:30</t>
   </si>
   <si>
-    <t>Break</t>
-  </si>
-  <si>
     <t>Intro to Apache Spark Workshop</t>
-  </si>
-  <si>
-    <t>Exercise 4 - Spark Submit</t>
   </si>
   <si>
     <r>
@@ -172,18 +136,6 @@
     <t>Apache Spark APIs</t>
   </si>
   <si>
-    <t>10:00 - 10:30</t>
-  </si>
-  <si>
-    <t>10:30 - 11:00</t>
-  </si>
-  <si>
-    <t>11:30 - 12:00</t>
-  </si>
-  <si>
-    <t>12:00 - 1:00</t>
-  </si>
-  <si>
     <t>1:00 - 1:30</t>
   </si>
   <si>
@@ -191,6 +143,42 @@
   </si>
   <si>
     <t>Exercise 1 - Running Spark Jobs</t>
+  </si>
+  <si>
+    <t>9:00 - 9:30</t>
+  </si>
+  <si>
+    <t>9:30 - 9:45</t>
+  </si>
+  <si>
+    <t>9:45 - 10:15</t>
+  </si>
+  <si>
+    <t>10:15 - 10:45</t>
+  </si>
+  <si>
+    <t>10:45 - 11:15</t>
+  </si>
+  <si>
+    <t>11:15 - 11:45</t>
+  </si>
+  <si>
+    <t>11:45 - 1:00</t>
+  </si>
+  <si>
+    <t>Advanced Apache Spark APIs and Lineage</t>
+  </si>
+  <si>
+    <t>3:00 - 3:15</t>
+  </si>
+  <si>
+    <t>Exercise 3 - Joining Datasets</t>
+  </si>
+  <si>
+    <t>Exercise 4 - Shared Variables</t>
+  </si>
+  <si>
+    <t>2:30 - 3:00</t>
   </si>
 </sst>
 </file>
@@ -736,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -749,14 +737,14 @@
   <sheetData>
     <row r="1" spans="1:3" ht="41" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="25" customHeight="1">
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C2" s="7"/>
     </row>
@@ -769,7 +757,7 @@
     </row>
     <row r="4" spans="1:3" ht="173" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -785,7 +773,7 @@
     </row>
     <row r="6" spans="1:3" ht="29" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
@@ -794,7 +782,7 @@
     </row>
     <row r="7" spans="1:3" ht="29" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
@@ -803,43 +791,43 @@
     </row>
     <row r="8" spans="1:3" ht="29" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="29" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="4" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="4" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="2" t="s">
@@ -848,80 +836,61 @@
     </row>
     <row r="13" spans="1:3" ht="29" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="29" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" customHeight="1">
-      <c r="A17" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="2" t="s">
-        <v>23</v>
+      <c r="A17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="29" customHeight="1">
-      <c r="A19" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="29" customHeight="1">
-      <c r="A20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A17:B17"/>
+  <mergeCells count="18">
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A11:B11"/>
@@ -930,8 +899,7 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A6:B6"/>

</xml_diff>